<commit_message>
Revert "20241026 차경환 사풍 용어 추가"
This reverts commit 7e35174f0b3a265dc997a5456c215860419535aa.
</commit_message>
<xml_diff>
--- a/기획/테이블/행로/행로 스트링 테이블.xlsx
+++ b/기획/테이블/행로/행로 스트링 테이블.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\addmin\Desktop\Unreal\UnrealProject\기획\테이블\행로\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB63164-3050-4FD5-B1F4-805E3E99C338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2985733-B871-4E4E-A621-4146FB6F07D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="2535" windowWidth="20220" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-270" yWindow="135" windowWidth="27405" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -167,15 +167,16 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>플레이어 캐릭터의 공격력이 20 증가한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>대지모와 소통하던 무당들의 행로. 아무리 위대하다한들 한낯 인간의 업적이다. 그것을 알기에 무당들은 석반에 매몰되지 않았고, 쇠락할지언정 끊어지진 않았다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>플레이어 캐릭터의 점성이 50 증가한다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>플레이어 캐릭터의 사풍이 20 증가한다.</t>
   </si>
 </sst>
 </file>
@@ -502,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -678,7 +679,7 @@
         <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -692,10 +693,10 @@
         <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>